<commit_message>
cargar vector propiedades y ventana Compras
</commit_message>
<xml_diff>
--- a/coordenadas.xlsx
+++ b/coordenadas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Monopoly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Desktop\Monopoly\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -72,7 +72,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -91,6 +91,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -104,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -113,6 +119,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -397,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E5:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,13 +421,13 @@
   </cols>
   <sheetData>
     <row r="5" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -455,18 +467,15 @@
       <c r="E7" s="1">
         <v>20160</v>
       </c>
-      <c r="H7">
-        <v>99895331</v>
-      </c>
       <c r="O7" s="1">
         <v>640160</v>
       </c>
     </row>
     <row r="8" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="1">
+      <c r="E8" s="4">
         <v>20215</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8" s="4">
         <v>640215</v>
       </c>
     </row>
@@ -490,7 +499,7 @@
       <c r="E11" s="1">
         <v>20385</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11" s="4">
         <v>640385</v>
       </c>
     </row>
@@ -506,7 +515,7 @@
       <c r="E13" s="1">
         <v>20495</v>
       </c>
-      <c r="O13" s="1">
+      <c r="O13" s="4">
         <v>640495</v>
       </c>
     </row>
@@ -519,7 +528,7 @@
       </c>
     </row>
     <row r="15" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="1">
+      <c r="E15" s="4">
         <v>20640</v>
       </c>
       <c r="F15" s="1">
@@ -528,7 +537,7 @@
       <c r="G15" s="1">
         <v>160640</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="4">
         <v>215640</v>
       </c>
       <c r="I15" s="1">
@@ -537,19 +546,19 @@
       <c r="J15" s="1">
         <v>325640</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="4">
         <v>385640</v>
       </c>
       <c r="L15" s="1">
         <v>440640</v>
       </c>
-      <c r="M15" s="1">
+      <c r="M15" s="4">
         <v>495640</v>
       </c>
       <c r="N15" s="1">
         <v>555640</v>
       </c>
-      <c r="O15" s="1">
+      <c r="O15" s="4">
         <v>640640</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lidiando con gets de propiedades
</commit_message>
<xml_diff>
--- a/coordenadas.xlsx
+++ b/coordenadas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Desktop\Monopoly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Monopoly\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E5:O15"/>
+  <dimension ref="D4:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,7 +432,27 @@
     <col min="15" max="15" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>14</v>
+      </c>
+      <c r="H4">
+        <v>15</v>
+      </c>
+      <c r="I4">
+        <v>16</v>
+      </c>
+      <c r="K4">
+        <v>18</v>
+      </c>
+      <c r="L4">
+        <v>19</v>
+      </c>
+      <c r="N4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="4:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" s="5" t="s">
         <v>0</v>
       </c>
@@ -467,23 +487,35 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>13</v>
+      </c>
       <c r="E6" s="6">
         <v>20105</v>
       </c>
       <c r="O6" s="6">
         <v>640105</v>
       </c>
-    </row>
-    <row r="7" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="4:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>12</v>
+      </c>
       <c r="E7" s="6">
         <v>20160</v>
       </c>
       <c r="O7" s="6">
         <v>640160</v>
       </c>
-    </row>
-    <row r="8" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="4:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E8" s="4">
         <v>20215</v>
       </c>
@@ -491,15 +523,21 @@
         <v>640215</v>
       </c>
     </row>
-    <row r="9" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>11</v>
+      </c>
       <c r="E9" s="6">
         <v>20270</v>
       </c>
       <c r="O9" s="6">
         <v>640270</v>
       </c>
-    </row>
-    <row r="10" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="4:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E10" s="1">
         <v>20325</v>
       </c>
@@ -507,7 +545,10 @@
         <v>640325</v>
       </c>
     </row>
-    <row r="11" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>9</v>
+      </c>
       <c r="E11" s="6">
         <v>20385</v>
       </c>
@@ -515,15 +556,21 @@
         <v>640385</v>
       </c>
     </row>
-    <row r="12" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>8</v>
+      </c>
       <c r="E12" s="6">
         <v>20440</v>
       </c>
       <c r="O12" s="6">
         <v>640440</v>
       </c>
-    </row>
-    <row r="13" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P12">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="4:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E13" s="1">
         <v>20495</v>
       </c>
@@ -531,15 +578,21 @@
         <v>640495</v>
       </c>
     </row>
-    <row r="14" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>6</v>
+      </c>
       <c r="E14" s="6">
         <v>20555</v>
       </c>
       <c r="O14" s="6">
         <v>640555</v>
       </c>
-    </row>
-    <row r="15" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="4:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E15" s="4">
         <v>20640</v>
       </c>
@@ -572,6 +625,23 @@
       </c>
       <c r="O15" s="4">
         <v>640640</v>
+      </c>
+    </row>
+    <row r="16" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregadas tarjetas de ferrocarriles
</commit_message>
<xml_diff>
--- a/coordenadas.xlsx
+++ b/coordenadas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Monopoly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Desktop\Monopoly\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -421,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,6 +442,9 @@
       <c r="I4">
         <v>16</v>
       </c>
+      <c r="J4">
+        <v>17</v>
+      </c>
       <c r="K4">
         <v>18</v>
       </c>
@@ -538,11 +541,17 @@
       </c>
     </row>
     <row r="10" spans="4:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>10</v>
+      </c>
       <c r="E10" s="1">
         <v>20325</v>
       </c>
       <c r="O10" s="1">
         <v>640325</v>
+      </c>
+      <c r="P10">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="4:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -636,6 +645,9 @@
       </c>
       <c r="I16">
         <v>3</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
       </c>
       <c r="L16">
         <v>1</v>

</xml_diff>

<commit_message>
funcion cobrar renta propiedades
</commit_message>
<xml_diff>
--- a/coordenadas.xlsx
+++ b/coordenadas.xlsx
@@ -116,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -137,6 +137,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -422,7 +425,7 @@
   <dimension ref="D4:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +483,7 @@
       <c r="L5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="8" t="s">
         <v>8</v>
       </c>
       <c r="N5" s="7" t="s">
@@ -658,5 +661,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
graficos y ventana hipotecar
</commit_message>
<xml_diff>
--- a/coordenadas.xlsx
+++ b/coordenadas.xlsx
@@ -424,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,6 +454,9 @@
       <c r="L4">
         <v>19</v>
       </c>
+      <c r="M4">
+        <v>20</v>
+      </c>
       <c r="N4">
         <v>21</v>
       </c>
@@ -583,6 +586,9 @@
       </c>
     </row>
     <row r="13" spans="4:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>7</v>
+      </c>
       <c r="E13" s="1">
         <v>20495</v>
       </c>

</xml_diff>

<commit_message>
cartas de arca y fortuna funcionando en un 90%
</commit_message>
<xml_diff>
--- a/coordenadas.xlsx
+++ b/coordenadas.xlsx
@@ -72,7 +72,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,6 +100,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -116,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -140,6 +158,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -424,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +495,7 @@
       <c r="F5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="10" t="s">
         <v>2</v>
       </c>
       <c r="H5" s="7" t="s">
@@ -525,10 +552,10 @@
       </c>
     </row>
     <row r="8" spans="4:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="4">
+      <c r="E8" s="9">
         <v>20215</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8" s="9">
         <v>640215</v>
       </c>
     </row>
@@ -567,7 +594,7 @@
       <c r="E11" s="6">
         <v>20385</v>
       </c>
-      <c r="O11" s="4">
+      <c r="O11" s="11">
         <v>640385</v>
       </c>
     </row>
@@ -620,7 +647,7 @@
       <c r="G15" s="6">
         <v>160640</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="11">
         <v>215640</v>
       </c>
       <c r="I15" s="6">
@@ -635,7 +662,7 @@
       <c r="L15" s="6">
         <v>440640</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15" s="9">
         <v>495640</v>
       </c>
       <c r="N15" s="6">

</xml_diff>